<commit_message>
Added more porewater data. Moved the pw calculation to a designated script, and created nice pw profile figure with both IC and colorimetric data.
</commit_message>
<xml_diff>
--- a/index/data/IC_raw_data.xlsx
+++ b/index/data/IC_raw_data.xlsx
@@ -8,17 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harmv\Documents\studie\scriptie\Master\Master_Thesis\index\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11B97571-5BCA-4E99-9AAD-B25701BB3470}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{519ADD57-3EA6-4477-A911-B454D2C0CD1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -2234,8 +2243,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L570"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A545" workbookViewId="0">
-      <selection activeCell="C359" sqref="C359"/>
+    <sheetView tabSelected="1" topLeftCell="A481" workbookViewId="0">
+      <selection activeCell="C355" sqref="C286:C355"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>